<commit_message>
Update sequence diagram and delete some function
</commit_message>
<xml_diff>
--- a/Lab1.3/Lab-1.3-Requirements Linkage Traceability Matrix.xlsx
+++ b/Lab1.3/Lab-1.3-Requirements Linkage Traceability Matrix.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giaba\OneDrive\Documents\GitHub\SE357-Pratice-class\Lab1.3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14205BA6-53DB-493F-9D07-B60FCA8ECA19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDAC7BE2-FE1F-45E9-8B55-D7DCA9A9C3A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{26FFCE25-151A-40F0-9F51-80939D4665D5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="57">
   <si>
     <t>Đăng nhập</t>
   </si>
@@ -92,12 +92,6 @@
     <t>Theo dõi tiến độ kế hoạch điều trị</t>
   </si>
   <si>
-    <t>CRUD hợp đồng dịch vụ</t>
-  </si>
-  <si>
-    <t>CRUD hợp đồng cung cấp vật tư</t>
-  </si>
-  <si>
     <t>CRUD  thông tin phòng khám</t>
   </si>
   <si>
@@ -123,9 +117,6 @@
   </si>
   <si>
     <t xml:space="preserve">CRUD lịch hẹn </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Xuất hóa đơn </t>
   </si>
   <si>
     <t>Acceptance Criteria</t>
@@ -148,9 +139,6 @@
 Tin nhắn phải được gửi và nhận một cách đáng tin cậy</t>
   </si>
   <si>
-    <t>Hệ thống có khả năng xuất hóa đơn cho viện phí và dịch vụ.</t>
-  </si>
-  <si>
     <t>Hệ thống phải có khả năng in hồ sơ bệnh án của bệnh nhân.</t>
   </si>
   <si>
@@ -206,12 +194,6 @@
   </si>
   <si>
     <t>Bác sĩ và bênh nhận khả năng theo dõi tiến độ kế hoạch điều trị của bệnh nhân.</t>
-  </si>
-  <si>
-    <t>Quản lí có thể thêm, sửa đổi, xóa thông tin về hợp đồng dịch vụ.</t>
-  </si>
-  <si>
-    <t>Quản lí có thể thêm, sửa đổi, xóa thông tin về hợp đồng cung cấp vật tư.</t>
   </si>
   <si>
     <t>Quản lí có thể thêm, sửa đổi, xóa thông tin về phòng khám.</t>
@@ -229,12 +211,18 @@
   <si>
     <t>Requirement</t>
   </si>
+  <si>
+    <t>CRUD thiết bị nha khoa</t>
+  </si>
+  <si>
+    <t>Quản lí có thể thêm, sửa đổi, xóa thông tin về thiết bị nha khoa</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -289,12 +277,6 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF1F1F1F"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -332,7 +314,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -358,7 +340,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -674,10 +663,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8854E2F-0770-4487-8904-2AC368AD1999}">
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" zoomScale="66" zoomScaleNormal="30" zoomScalePageLayoutView="66" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" topLeftCell="A8" zoomScale="66" zoomScaleNormal="30" zoomScalePageLayoutView="66" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -695,19 +684,19 @@
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -722,13 +711,13 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="F2" s="1"/>
     </row>
@@ -740,13 +729,13 @@
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="F3" s="1"/>
     </row>
@@ -758,13 +747,13 @@
         <v>2</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="F4" s="1"/>
     </row>
@@ -776,13 +765,13 @@
         <v>3</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="F5" s="1"/>
     </row>
@@ -794,13 +783,13 @@
         <v>4</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="F6" s="1"/>
     </row>
@@ -812,13 +801,13 @@
         <v>5</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="64.5" x14ac:dyDescent="0.25">
@@ -826,16 +815,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="64.5" x14ac:dyDescent="0.25">
@@ -843,16 +832,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="64.5" x14ac:dyDescent="0.25">
@@ -860,16 +849,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="64.5" x14ac:dyDescent="0.25">
@@ -877,16 +866,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>24</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="64.5" x14ac:dyDescent="0.25">
@@ -894,16 +883,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="64.5" x14ac:dyDescent="0.25">
@@ -911,16 +900,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="64.5" x14ac:dyDescent="0.25">
@@ -928,16 +917,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>24</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="64.5" x14ac:dyDescent="0.25">
@@ -945,16 +934,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="64.5" x14ac:dyDescent="0.25">
@@ -962,16 +951,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="64.5" x14ac:dyDescent="0.25">
@@ -979,16 +968,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="64.5" x14ac:dyDescent="0.25">
@@ -996,16 +985,16 @@
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>24</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="64.5" x14ac:dyDescent="0.25">
@@ -1013,16 +1002,16 @@
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="64.5" x14ac:dyDescent="0.25">
@@ -1030,16 +1019,16 @@
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="64.5" x14ac:dyDescent="0.25">
@@ -1047,16 +1036,16 @@
         <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C21" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D21" s="8" t="s">
-        <v>51</v>
+      <c r="D21" s="10" t="s">
+        <v>48</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="64.5" x14ac:dyDescent="0.25">
@@ -1064,16 +1053,16 @@
         <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>52</v>
+        <v>16</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>49</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="64.5" x14ac:dyDescent="0.25">
@@ -1081,16 +1070,16 @@
         <v>22</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="64.5" x14ac:dyDescent="0.25">
@@ -1098,67 +1087,33 @@
         <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C24" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="64.5" x14ac:dyDescent="0.25">
+      <c r="A25" s="11">
         <v>24</v>
       </c>
-      <c r="D24" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="E24" s="7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="64.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="5">
-        <v>24</v>
-      </c>
-      <c r="B25" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D25" s="8" t="s">
+      <c r="B25" s="12" t="s">
         <v>55</v>
       </c>
+      <c r="C25" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>56</v>
+      </c>
       <c r="E25" s="7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="64.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="5">
-        <v>25</v>
-      </c>
-      <c r="B26" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="E26" s="7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="64.5" x14ac:dyDescent="0.25">
-      <c r="A27" s="5">
-        <v>26</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="E27" s="7" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>